<commit_message>
reconfigure adworks lt data layout
</commit_message>
<xml_diff>
--- a/ad_works_lt/pipelines/tables.xlsx
+++ b/ad_works_lt/pipelines/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/databricks-patterns/ad_works_lt/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3D8B5E-3E01-004A-AC1B-D77CF4E4E658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4ED61D-68C6-E146-83E7-70856806BECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1240" windowWidth="38400" windowHeight="21100" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,15 +179,6 @@
     <t>sales_order_header</t>
   </si>
   <si>
-    <t>landing_ad_works_lt</t>
-  </si>
-  <si>
-    <t>control_ad_works_lt</t>
-  </si>
-  <si>
-    <t>raw_ad_works_lt</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
@@ -212,73 +203,82 @@
 SalesOrderNumber</t>
   </si>
   <si>
-    <t>landing.landing_ad_works_lt.address</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.customer</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.customer_address</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.product</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.product_category</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.product_description</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.product_model</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.product_model_product_description</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.sales_order_detail</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_lt.sales_order_header</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.address</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.customer</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.customer_address</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.product</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.product_category</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.product_description</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.product_model</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.product_model_product_description</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.sales_order_detail</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works_lt.sales_order_header</t>
-  </si>
-  <si>
     <t>base_audit</t>
   </si>
   <si>
     <t>base.raw_ad_works.*</t>
   </si>
   <si>
-    <t>base_ad_works_lt</t>
+    <t>yetl_control_ad_works_lt</t>
+  </si>
+  <si>
+    <t>yetl_landing_ad_works_lt</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.address</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.customer</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.customer_address</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.product</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.product_category</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.product_description</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.product_model</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.product_model_product_description</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.sales_order_detail</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works_lt.sales_order_header</t>
+  </si>
+  <si>
+    <t>yetl_raw_ad_works_lt</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.address</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.customer</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.customer_address</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.product</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.product_category</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.product_description</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.product_model</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.product_model_product_description</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.sales_order_detail</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.sales_order_header</t>
+  </si>
+  <si>
+    <t>yetl_base_ad_works_lt</t>
   </si>
 </sst>
 </file>
@@ -446,16 +446,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -781,7 +781,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,25 +814,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="25" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="27" t="s">
@@ -843,31 +843,31 @@
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="25" t="s">
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
       <c r="V1" s="28" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="28"/>
     </row>
     <row r="2" spans="1:24" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="11" t="s">
         <v>21</v>
       </c>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
@@ -965,17 +965,17 @@
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1005,7 +1005,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>37</v>
@@ -1020,7 +1020,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>38</v>
@@ -1034,7 +1034,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>39</v>
@@ -1048,7 +1048,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>40</v>
@@ -1062,7 +1062,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>41</v>
@@ -1076,7 +1076,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>42</v>
@@ -1090,7 +1090,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>43</v>
@@ -1104,7 +1104,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>44</v>
@@ -1118,7 +1118,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>45</v>
@@ -1132,7 +1132,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>46</v>
@@ -1146,7 +1146,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
@@ -1155,7 +1155,7 @@
         <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>25</v>
@@ -1184,7 +1184,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>38</v>
@@ -1194,7 +1194,7 @@
         <v>36</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>25</v>
@@ -1223,17 +1223,17 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>25</v>
@@ -1262,17 +1262,17 @@
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>25</v>
@@ -1301,7 +1301,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>41</v>
@@ -1311,7 +1311,7 @@
         <v>33</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>25</v>
@@ -1340,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>42</v>
@@ -1350,7 +1350,7 @@
         <v>34</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>25</v>
@@ -1379,7 +1379,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>43</v>
@@ -1389,7 +1389,7 @@
         <v>35</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>25</v>
@@ -1418,17 +1418,17 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>25</v>
@@ -1457,17 +1457,17 @@
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>25</v>
@@ -1496,17 +1496,17 @@
         <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>25</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="25" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>14</v>
@@ -1545,7 +1545,7 @@
         <v>32</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="6">
@@ -1566,7 +1566,7 @@
     </row>
     <row r="26" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>14</v>
@@ -1582,7 +1582,7 @@
         <v>36</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="6">
@@ -1603,7 +1603,7 @@
     </row>
     <row r="27" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
@@ -1616,10 +1616,10 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="6">
@@ -1640,7 +1640,7 @@
     </row>
     <row r="28" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>14</v>
@@ -1653,10 +1653,10 @@
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="6">
@@ -1677,7 +1677,7 @@
     </row>
     <row r="29" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
@@ -1693,7 +1693,7 @@
         <v>33</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="6">
@@ -1714,7 +1714,7 @@
     </row>
     <row r="30" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>14</v>
@@ -1730,7 +1730,7 @@
         <v>34</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="6">
@@ -1751,7 +1751,7 @@
     </row>
     <row r="31" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>14</v>
@@ -1767,7 +1767,7 @@
         <v>35</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="6">
@@ -1788,7 +1788,7 @@
     </row>
     <row r="32" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>14</v>
@@ -1801,10 +1801,10 @@
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="6">
@@ -1825,7 +1825,7 @@
     </row>
     <row r="33" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>14</v>
@@ -1838,10 +1838,10 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="6">
@@ -1862,7 +1862,7 @@
     </row>
     <row r="34" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>14</v>
@@ -1875,10 +1875,10 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="6">
@@ -2350,17 +2350,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="V1:W1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
reconfigure adworks lt data clear
</commit_message>
<xml_diff>
--- a/ad_works_lt/pipelines/tables.xlsx
+++ b/ad_works_lt/pipelines/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/databricks-patterns/ad_works_lt/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4ED61D-68C6-E146-83E7-70856806BECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F087668-9BC2-D74F-95A1-485C58592D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>vacuum</t>
   </si>
   <si>
-    <t>raw.raw_ad_works.*</t>
-  </si>
-  <si>
     <t>AddressID</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>base_audit</t>
   </si>
   <si>
-    <t>base.raw_ad_works.*</t>
-  </si>
-  <si>
     <t>yetl_control_ad_works_lt</t>
   </si>
   <si>
@@ -279,6 +273,12 @@
   </si>
   <si>
     <t>yetl_base_ad_works_lt</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works_lt.*</t>
+  </si>
+  <si>
+    <t>base.yetl_base_ad_works_lt.*</t>
   </si>
 </sst>
 </file>
@@ -781,7 +781,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
@@ -935,7 +935,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -965,17 +965,17 @@
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1005,10 +1005,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -1020,10 +1020,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1034,10 +1034,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1048,10 +1048,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1062,10 +1062,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1076,10 +1076,10 @@
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1090,10 +1090,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1104,10 +1104,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1118,10 +1118,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1132,10 +1132,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1146,16 +1146,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>25</v>
@@ -1184,17 +1184,17 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>25</v>
@@ -1223,17 +1223,17 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>25</v>
@@ -1262,17 +1262,17 @@
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>25</v>
@@ -1301,17 +1301,17 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>25</v>
@@ -1340,17 +1340,17 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>25</v>
@@ -1379,17 +1379,17 @@
         <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>25</v>
@@ -1418,17 +1418,17 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>25</v>
@@ -1457,17 +1457,17 @@
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>25</v>
@@ -1496,17 +1496,17 @@
         <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>25</v>
@@ -1529,23 +1529,23 @@
     </row>
     <row r="25" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="6">
@@ -1566,23 +1566,23 @@
     </row>
     <row r="26" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="6">
@@ -1603,23 +1603,23 @@
     </row>
     <row r="27" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="6">
@@ -1640,23 +1640,23 @@
     </row>
     <row r="28" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="6">
@@ -1677,23 +1677,23 @@
     </row>
     <row r="29" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="6">
@@ -1714,23 +1714,23 @@
     </row>
     <row r="30" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="6">
@@ -1751,23 +1751,23 @@
     </row>
     <row r="31" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="6">
@@ -1788,23 +1788,23 @@
     </row>
     <row r="32" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="6">
@@ -1825,23 +1825,23 @@
     </row>
     <row r="33" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="6">
@@ -1862,23 +1862,23 @@
     </row>
     <row r="34" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="6">

</xml_diff>

<commit_message>
ad works lt onto catalog
</commit_message>
<xml_diff>
--- a/ad_works_lt/pipelines/tables.xlsx
+++ b/ad_works_lt/pipelines/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/databricks-patterns/ad_works_lt/pipelines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/python/databricks-patterns/ad_works_lt/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4833CA08-BFA3-3548-8A2F-1FCF457489B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1E8F17-3A1A-A444-A0F9-96781CAC2665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
+    <workbookView xWindow="-38400" yWindow="1240" windowWidth="38400" windowHeight="21100" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="82">
   <si>
     <t>stage</t>
   </si>
@@ -197,84 +197,6 @@
     <t>base_audit</t>
   </si>
   <si>
-    <t>yetl_control_ad_works_lt</t>
-  </si>
-  <si>
-    <t>yetl_landing_ad_works_lt</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.address</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.customer</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.customer_address</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.product</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.product_category</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.product_description</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.product_model</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.product_model_product_description</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.sales_order_detail</t>
-  </si>
-  <si>
-    <t>landing.yetl_landing_ad_works_lt.sales_order_header</t>
-  </si>
-  <si>
-    <t>yetl_raw_ad_works_lt</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.address</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.customer</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.customer_address</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.product</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.product_category</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.product_description</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.product_model</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.product_model_product_description</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.sales_order_detail</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.sales_order_header</t>
-  </si>
-  <si>
-    <t>yetl_base_ad_works_lt</t>
-  </si>
-  <si>
-    <t>raw.yetl_raw_ad_works_lt.*</t>
-  </si>
-  <si>
-    <t>base.yetl_base_ad_works_lt.*</t>
-  </si>
-  <si>
     <t>catalog</t>
   </si>
   <si>
@@ -282,6 +204,90 @@
   </si>
   <si>
     <t>exception_thresholds</t>
+  </si>
+  <si>
+    <t>control_ad_works_lt</t>
+  </si>
+  <si>
+    <t>landing_ad_works_lt</t>
+  </si>
+  <si>
+    <t>raw_ad_works_lt</t>
+  </si>
+  <si>
+    <t>base_ad_works_lt</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.*</t>
+  </si>
+  <si>
+    <t>base.base_ad_works_lt.*</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.address</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.customer</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.customer_address</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.product</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.product_category</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.product_description</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.product_model</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.product_model_product_description</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.sales_order_detail</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_lt.sales_order_header</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.address</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.customer</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.customer_address</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.product</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.product_category</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.product_description</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.product_model</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.product_model_product_description</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.sales_order_detail</t>
+  </si>
+  <si>
+    <t>raw.raw_ad_works_lt.sales_order_header</t>
+  </si>
+  <si>
+    <t>cluster_by</t>
+  </si>
+  <si>
+    <t>development</t>
   </si>
 </sst>
 </file>
@@ -435,16 +441,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -766,18 +772,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
-  <dimension ref="A1:Y83"/>
+  <dimension ref="A1:Z83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.5" style="2" bestFit="1" customWidth="1"/>
@@ -786,46 +792,47 @@
     <col min="9" max="9" width="34.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="16" style="2"/>
+    <col min="12" max="12" width="11" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="16" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="26" t="s">
@@ -836,32 +843,33 @@
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="27" t="s">
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="27"/>
-    </row>
-    <row r="2" spans="1:25" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="Y1" s="27"/>
+    </row>
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="10" t="s">
         <v>19</v>
       </c>
@@ -872,55 +880,60 @@
         <v>26</v>
       </c>
       <c r="L2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="S2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="W2" s="11" t="s">
+      <c r="W2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="Y2" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
@@ -930,38 +943,41 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="6">
+      <c r="N3" s="3"/>
+      <c r="O3" s="6">
         <v>30</v>
       </c>
-      <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="7"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="5"/>
-    </row>
-    <row r="4" spans="1:25" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="W3" s="5"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>50</v>
@@ -971,189 +987,212 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="6">
+      <c r="N4" s="3"/>
+      <c r="O4" s="6">
         <v>30</v>
       </c>
-      <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="7"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="5"/>
-    </row>
-    <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="W4" s="5"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D9" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D11" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>34</v>
@@ -1162,37 +1201,39 @@
         <v>29</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="6">
+      <c r="O15" s="6">
         <v>30</v>
       </c>
-      <c r="T15" s="2">
+      <c r="U15" s="2">
         <v>0</v>
       </c>
-      <c r="V15" s="2">
-        <v>1</v>
-      </c>
-      <c r="W15" s="17">
-        <v>1</v>
-      </c>
-      <c r="X15" s="15">
+      <c r="W15" s="2">
+        <v>1</v>
+      </c>
+      <c r="X15" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D16" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>35</v>
@@ -1202,37 +1243,39 @@
         <v>33</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="6">
+      <c r="O16" s="6">
         <v>30</v>
       </c>
-      <c r="T16" s="2">
+      <c r="U16" s="2">
         <v>0</v>
       </c>
-      <c r="V16" s="2">
-        <v>1</v>
-      </c>
-      <c r="W16" s="17">
-        <v>1</v>
-      </c>
-      <c r="X16" s="15">
+      <c r="W16" s="2">
+        <v>1</v>
+      </c>
+      <c r="X16" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D17" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>36</v>
@@ -1242,37 +1285,39 @@
         <v>45</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N17" s="6">
+      <c r="O17" s="6">
         <v>30</v>
       </c>
-      <c r="T17" s="2">
+      <c r="U17" s="2">
         <v>0</v>
       </c>
-      <c r="V17" s="2">
-        <v>1</v>
-      </c>
-      <c r="W17" s="17">
-        <v>1</v>
-      </c>
-      <c r="X17" s="15">
+      <c r="W17" s="2">
+        <v>1</v>
+      </c>
+      <c r="X17" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D18" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>37</v>
@@ -1282,37 +1327,39 @@
         <v>46</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N18" s="6">
+      <c r="O18" s="6">
         <v>30</v>
       </c>
-      <c r="T18" s="2">
+      <c r="U18" s="2">
         <v>0</v>
       </c>
-      <c r="V18" s="2">
-        <v>1</v>
-      </c>
-      <c r="W18" s="17">
-        <v>1</v>
-      </c>
-      <c r="X18" s="15">
+      <c r="W18" s="2">
+        <v>1</v>
+      </c>
+      <c r="X18" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D19" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>38</v>
@@ -1322,37 +1369,39 @@
         <v>30</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="6">
+      <c r="O19" s="6">
         <v>30</v>
       </c>
-      <c r="T19" s="2">
+      <c r="U19" s="2">
         <v>0</v>
       </c>
-      <c r="V19" s="2">
-        <v>1</v>
-      </c>
-      <c r="W19" s="17">
-        <v>1</v>
-      </c>
-      <c r="X19" s="15">
+      <c r="W19" s="2">
+        <v>1</v>
+      </c>
+      <c r="X19" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D20" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>39</v>
@@ -1362,37 +1411,39 @@
         <v>31</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="6">
+      <c r="O20" s="6">
         <v>30</v>
       </c>
-      <c r="T20" s="2">
+      <c r="U20" s="2">
         <v>0</v>
       </c>
-      <c r="V20" s="2">
-        <v>1</v>
-      </c>
-      <c r="W20" s="17">
-        <v>1</v>
-      </c>
-      <c r="X20" s="15">
+      <c r="W20" s="2">
+        <v>1</v>
+      </c>
+      <c r="X20" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D21" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>40</v>
@@ -1402,37 +1453,39 @@
         <v>32</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N21" s="6">
+      <c r="O21" s="6">
         <v>30</v>
       </c>
-      <c r="T21" s="2">
+      <c r="U21" s="2">
         <v>0</v>
       </c>
-      <c r="V21" s="2">
-        <v>1</v>
-      </c>
-      <c r="W21" s="17">
-        <v>1</v>
-      </c>
-      <c r="X21" s="15">
+      <c r="W21" s="2">
+        <v>1</v>
+      </c>
+      <c r="X21" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D22" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>41</v>
@@ -1442,37 +1495,39 @@
         <v>47</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N22" s="6">
+      <c r="O22" s="6">
         <v>30</v>
       </c>
-      <c r="T22" s="2">
+      <c r="U22" s="2">
         <v>0</v>
       </c>
-      <c r="V22" s="2">
-        <v>1</v>
-      </c>
-      <c r="W22" s="17">
-        <v>1</v>
-      </c>
-      <c r="X22" s="15">
+      <c r="W22" s="2">
+        <v>1</v>
+      </c>
+      <c r="X22" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>42</v>
@@ -1482,37 +1537,39 @@
         <v>48</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N23" s="6">
+      <c r="O23" s="6">
         <v>30</v>
       </c>
-      <c r="T23" s="2">
+      <c r="U23" s="2">
         <v>0</v>
       </c>
-      <c r="V23" s="2">
-        <v>1</v>
-      </c>
-      <c r="W23" s="17">
-        <v>1</v>
-      </c>
-      <c r="X23" s="15">
+      <c r="W23" s="2">
+        <v>1</v>
+      </c>
+      <c r="X23" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D24" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>43</v>
@@ -1522,37 +1579,39 @@
         <v>49</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="6">
+      <c r="O24" s="6">
         <v>30</v>
       </c>
-      <c r="T24" s="2">
+      <c r="U24" s="2">
         <v>0</v>
       </c>
-      <c r="V24" s="2">
-        <v>1</v>
-      </c>
-      <c r="W24" s="17">
-        <v>1</v>
-      </c>
-      <c r="X24" s="15">
+      <c r="W24" s="2">
+        <v>1</v>
+      </c>
+      <c r="X24" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D25" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>34</v>
@@ -1562,35 +1621,37 @@
         <v>29</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M25" s="3"/>
-      <c r="N25" s="6">
+        <v>70</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="6">
         <v>30</v>
       </c>
-      <c r="T25" s="2">
+      <c r="U25" s="2">
         <v>0</v>
       </c>
-      <c r="V25" s="2">
-        <v>1</v>
-      </c>
-      <c r="W25" s="17">
-        <v>1</v>
-      </c>
-      <c r="X25" s="15">
+      <c r="W25" s="2">
+        <v>1</v>
+      </c>
+      <c r="X25" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D26" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>35</v>
@@ -1600,35 +1661,37 @@
         <v>33</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M26" s="3"/>
-      <c r="N26" s="6">
+        <v>71</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="6">
         <v>30</v>
       </c>
-      <c r="T26" s="2">
+      <c r="U26" s="2">
         <v>0</v>
       </c>
-      <c r="V26" s="2">
-        <v>1</v>
-      </c>
-      <c r="W26" s="17">
-        <v>1</v>
-      </c>
-      <c r="X26" s="15">
+      <c r="W26" s="2">
+        <v>1</v>
+      </c>
+      <c r="X26" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D27" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>36</v>
@@ -1638,35 +1701,37 @@
         <v>45</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M27" s="3"/>
-      <c r="N27" s="6">
+        <v>72</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="6">
         <v>30</v>
       </c>
-      <c r="T27" s="2">
+      <c r="U27" s="2">
         <v>0</v>
       </c>
-      <c r="V27" s="2">
-        <v>1</v>
-      </c>
-      <c r="W27" s="17">
-        <v>1</v>
-      </c>
-      <c r="X27" s="15">
+      <c r="W27" s="2">
+        <v>1</v>
+      </c>
+      <c r="X27" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D28" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>37</v>
@@ -1676,35 +1741,37 @@
         <v>46</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M28" s="3"/>
-      <c r="N28" s="6">
+        <v>73</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="6">
         <v>30</v>
       </c>
-      <c r="T28" s="2">
+      <c r="U28" s="2">
         <v>0</v>
       </c>
-      <c r="V28" s="2">
-        <v>1</v>
-      </c>
-      <c r="W28" s="17">
-        <v>1</v>
-      </c>
-      <c r="X28" s="15">
+      <c r="W28" s="2">
+        <v>1</v>
+      </c>
+      <c r="X28" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D29" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>38</v>
@@ -1714,35 +1781,37 @@
         <v>30</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="6">
+        <v>74</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="6">
         <v>30</v>
       </c>
-      <c r="T29" s="2">
+      <c r="U29" s="2">
         <v>0</v>
       </c>
-      <c r="V29" s="2">
-        <v>1</v>
-      </c>
-      <c r="W29" s="17">
-        <v>1</v>
-      </c>
-      <c r="X29" s="15">
+      <c r="W29" s="2">
+        <v>1</v>
+      </c>
+      <c r="X29" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D30" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>39</v>
@@ -1752,35 +1821,37 @@
         <v>31</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="6">
+        <v>75</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="6">
         <v>30</v>
       </c>
-      <c r="T30" s="2">
+      <c r="U30" s="2">
         <v>0</v>
       </c>
-      <c r="V30" s="2">
-        <v>1</v>
-      </c>
-      <c r="W30" s="17">
-        <v>1</v>
-      </c>
-      <c r="X30" s="15">
+      <c r="W30" s="2">
+        <v>1</v>
+      </c>
+      <c r="X30" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D31" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>40</v>
@@ -1790,35 +1861,37 @@
         <v>32</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="6">
+        <v>76</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="6">
         <v>30</v>
       </c>
-      <c r="T31" s="2">
+      <c r="U31" s="2">
         <v>0</v>
       </c>
-      <c r="V31" s="2">
-        <v>1</v>
-      </c>
-      <c r="W31" s="17">
-        <v>1</v>
-      </c>
-      <c r="X31" s="15">
+      <c r="W31" s="2">
+        <v>1</v>
+      </c>
+      <c r="X31" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D32" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>41</v>
@@ -1828,35 +1901,37 @@
         <v>47</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M32" s="3"/>
-      <c r="N32" s="6">
+        <v>77</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="6">
         <v>30</v>
       </c>
-      <c r="T32" s="2">
+      <c r="U32" s="2">
         <v>0</v>
       </c>
-      <c r="V32" s="2">
-        <v>1</v>
-      </c>
-      <c r="W32" s="17">
-        <v>1</v>
-      </c>
-      <c r="X32" s="15">
+      <c r="W32" s="2">
+        <v>1</v>
+      </c>
+      <c r="X32" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D33" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>42</v>
@@ -1866,35 +1941,37 @@
         <v>48</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M33" s="3"/>
-      <c r="N33" s="6">
+        <v>78</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="6">
         <v>30</v>
       </c>
-      <c r="T33" s="2">
+      <c r="U33" s="2">
         <v>0</v>
       </c>
-      <c r="V33" s="2">
-        <v>1</v>
-      </c>
-      <c r="W33" s="17">
-        <v>1</v>
-      </c>
-      <c r="X33" s="15">
+      <c r="W33" s="2">
+        <v>1</v>
+      </c>
+      <c r="X33" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D34" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>43</v>
@@ -1904,498 +1981,498 @@
         <v>49</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M34" s="3"/>
-      <c r="N34" s="6">
+        <v>79</v>
+      </c>
+      <c r="N34" s="3"/>
+      <c r="O34" s="6">
         <v>30</v>
       </c>
-      <c r="T34" s="2">
+      <c r="U34" s="2">
         <v>0</v>
       </c>
-      <c r="V34" s="2">
-        <v>1</v>
-      </c>
-      <c r="W34" s="17">
-        <v>1</v>
-      </c>
-      <c r="X34" s="15">
+      <c r="W34" s="2">
+        <v>1</v>
+      </c>
+      <c r="X34" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="15">
         <v>365</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="20"/>
       <c r="G35" s="18"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="6"/>
-      <c r="W35" s="17"/>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N35" s="3"/>
+      <c r="O35" s="6"/>
+      <c r="X35" s="17"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="20"/>
       <c r="G36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="6"/>
-      <c r="W36" s="17"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N36" s="3"/>
+      <c r="O36" s="6"/>
+      <c r="X36" s="17"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="20"/>
       <c r="G37" s="18"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="6"/>
-      <c r="W37" s="17"/>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N37" s="3"/>
+      <c r="O37" s="6"/>
+      <c r="X37" s="17"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="20"/>
       <c r="G38" s="18"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="6"/>
-      <c r="W38" s="17"/>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N38" s="3"/>
+      <c r="O38" s="6"/>
+      <c r="X38" s="17"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="20"/>
       <c r="G39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="6"/>
-      <c r="W39" s="17"/>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N39" s="3"/>
+      <c r="O39" s="6"/>
+      <c r="X39" s="17"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="20"/>
       <c r="G40" s="18"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="6"/>
-      <c r="W40" s="17"/>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N40" s="3"/>
+      <c r="O40" s="6"/>
+      <c r="X40" s="17"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="20"/>
       <c r="G41" s="19"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="6"/>
-      <c r="W41" s="17"/>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N41" s="3"/>
+      <c r="O41" s="6"/>
+      <c r="X41" s="17"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="20"/>
       <c r="G42" s="19"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="6"/>
-      <c r="W42" s="17"/>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N42" s="3"/>
+      <c r="O42" s="6"/>
+      <c r="X42" s="17"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="20"/>
       <c r="G43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="6"/>
-      <c r="W43" s="17"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N43" s="3"/>
+      <c r="O43" s="6"/>
+      <c r="X43" s="17"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="20"/>
       <c r="G44" s="18"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="6"/>
-      <c r="W44" s="17"/>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N44" s="3"/>
+      <c r="O44" s="6"/>
+      <c r="X44" s="17"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="20"/>
       <c r="G45" s="19"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="6"/>
-      <c r="W45" s="17"/>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N45" s="3"/>
+      <c r="O45" s="6"/>
+      <c r="X45" s="17"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="20"/>
       <c r="G46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="6"/>
-      <c r="W46" s="17"/>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N46" s="3"/>
+      <c r="O46" s="6"/>
+      <c r="X46" s="17"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="20"/>
       <c r="G47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="6"/>
-      <c r="W47" s="17"/>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N47" s="3"/>
+      <c r="O47" s="6"/>
+      <c r="X47" s="17"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="20"/>
       <c r="G48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="6"/>
-      <c r="W48" s="17"/>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N48" s="3"/>
+      <c r="O48" s="6"/>
+      <c r="X48" s="17"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="20"/>
       <c r="G49" s="18"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="6"/>
-      <c r="W49" s="17"/>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N49" s="3"/>
+      <c r="O49" s="6"/>
+      <c r="X49" s="17"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="20"/>
       <c r="G50" s="18"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="6"/>
-      <c r="W50" s="17"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N50" s="3"/>
+      <c r="O50" s="6"/>
+      <c r="X50" s="17"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="20"/>
       <c r="G51" s="18"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="6"/>
-      <c r="W51" s="17"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N51" s="3"/>
+      <c r="O51" s="6"/>
+      <c r="X51" s="17"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="20"/>
       <c r="G52" s="18"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="6"/>
-      <c r="W52" s="17"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N52" s="3"/>
+      <c r="O52" s="6"/>
+      <c r="X52" s="17"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="20"/>
       <c r="G53" s="18"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="6"/>
-      <c r="W53" s="17"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N53" s="3"/>
+      <c r="O53" s="6"/>
+      <c r="X53" s="17"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="20"/>
       <c r="G54" s="18"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="6"/>
-      <c r="W54" s="17"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N54" s="3"/>
+      <c r="O54" s="6"/>
+      <c r="X54" s="17"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="20"/>
       <c r="G55" s="18"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="6"/>
-      <c r="W55" s="17"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N55" s="3"/>
+      <c r="O55" s="6"/>
+      <c r="X55" s="17"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="20"/>
       <c r="G56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="6"/>
-      <c r="W56" s="17"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N56" s="3"/>
+      <c r="O56" s="6"/>
+      <c r="X56" s="17"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="20"/>
       <c r="G57" s="18"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="6"/>
-      <c r="W57" s="17"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N57" s="3"/>
+      <c r="O57" s="6"/>
+      <c r="X57" s="17"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="20"/>
       <c r="G58" s="19"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="6"/>
-      <c r="W58" s="17"/>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N58" s="3"/>
+      <c r="O58" s="6"/>
+      <c r="X58" s="17"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="20"/>
       <c r="G59" s="18"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="6"/>
-      <c r="W59" s="17"/>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N59" s="3"/>
+      <c r="O59" s="6"/>
+      <c r="X59" s="17"/>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="20"/>
       <c r="G60" s="18"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="6"/>
-      <c r="W60" s="17"/>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N60" s="3"/>
+      <c r="O60" s="6"/>
+      <c r="X60" s="17"/>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="20"/>
       <c r="G61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="6"/>
-      <c r="W61" s="17"/>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N61" s="3"/>
+      <c r="O61" s="6"/>
+      <c r="X61" s="17"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="20"/>
       <c r="G62" s="19"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="6"/>
-      <c r="W62" s="17"/>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N62" s="3"/>
+      <c r="O62" s="6"/>
+      <c r="X62" s="17"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="20"/>
       <c r="G63" s="18"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="6"/>
-      <c r="W63" s="17"/>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N63" s="3"/>
+      <c r="O63" s="6"/>
+      <c r="X63" s="17"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="20"/>
       <c r="G64" s="18"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="6"/>
-      <c r="W64" s="17"/>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N64" s="3"/>
+      <c r="O64" s="6"/>
+      <c r="X64" s="17"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="20"/>
       <c r="G65" s="18"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="6"/>
-      <c r="W65" s="17"/>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N65" s="3"/>
+      <c r="O65" s="6"/>
+      <c r="X65" s="17"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="20"/>
       <c r="G66" s="18"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="6"/>
-      <c r="W66" s="17"/>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N66" s="3"/>
+      <c r="O66" s="6"/>
+      <c r="X66" s="17"/>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="20"/>
       <c r="G67" s="19"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="6"/>
-      <c r="W67" s="17"/>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N67" s="3"/>
+      <c r="O67" s="6"/>
+      <c r="X67" s="17"/>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="20"/>
       <c r="G68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="6"/>
-      <c r="W68" s="17"/>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N68" s="3"/>
+      <c r="O68" s="6"/>
+      <c r="X68" s="17"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="20"/>
       <c r="G69" s="3"/>
-      <c r="M69" s="3"/>
-      <c r="N69" s="6"/>
-      <c r="W69" s="17"/>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N69" s="3"/>
+      <c r="O69" s="6"/>
+      <c r="X69" s="17"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="20"/>
       <c r="G70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="6"/>
-      <c r="W70" s="17"/>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N70" s="3"/>
+      <c r="O70" s="6"/>
+      <c r="X70" s="17"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="20"/>
       <c r="G71" s="18"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="6"/>
-      <c r="W71" s="17"/>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N71" s="3"/>
+      <c r="O71" s="6"/>
+      <c r="X71" s="17"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="20"/>
       <c r="G72" s="19"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="6"/>
-      <c r="W72" s="17"/>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N72" s="3"/>
+      <c r="O72" s="6"/>
+      <c r="X72" s="17"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="20"/>
       <c r="G73" s="18"/>
-      <c r="M73" s="3"/>
-      <c r="N73" s="6"/>
-      <c r="W73" s="17"/>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N73" s="3"/>
+      <c r="O73" s="6"/>
+      <c r="X73" s="17"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="20"/>
       <c r="G74" s="18"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="6"/>
-      <c r="W74" s="17"/>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N74" s="3"/>
+      <c r="O74" s="6"/>
+      <c r="X74" s="17"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="20"/>
       <c r="G75" s="18"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="6"/>
-      <c r="W75" s="17"/>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N75" s="3"/>
+      <c r="O75" s="6"/>
+      <c r="X75" s="17"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="20"/>
       <c r="G76" s="19"/>
-      <c r="M76" s="3"/>
-      <c r="N76" s="6"/>
-      <c r="W76" s="17"/>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N76" s="3"/>
+      <c r="O76" s="6"/>
+      <c r="X76" s="17"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="20"/>
       <c r="G77" s="18"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="6"/>
-      <c r="W77" s="17"/>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N77" s="3"/>
+      <c r="O77" s="6"/>
+      <c r="X77" s="17"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="20"/>
       <c r="G78" s="18"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="6"/>
-      <c r="W78" s="17"/>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N78" s="3"/>
+      <c r="O78" s="6"/>
+      <c r="X78" s="17"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="20"/>
       <c r="G79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="6"/>
-      <c r="W79" s="17"/>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N79" s="3"/>
+      <c r="O79" s="6"/>
+      <c r="X79" s="17"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="20"/>
       <c r="G80" s="18"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="6"/>
-      <c r="W80" s="17"/>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="N80" s="3"/>
+      <c r="O80" s="6"/>
+      <c r="X80" s="17"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="20"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="6"/>
-      <c r="W81" s="17"/>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="N81" s="3"/>
+      <c r="O81" s="6"/>
+      <c r="X81" s="17"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="G82" s="3"/>
     </row>
-    <row r="83" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -2409,26 +2486,22 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
       <c r="M83" s="3"/>
-      <c r="N83" s="6"/>
+      <c r="N83" s="3"/>
       <c r="O83" s="6"/>
       <c r="P83" s="6"/>
       <c r="Q83" s="6"/>
-      <c r="R83" s="8"/>
-      <c r="S83" s="6"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="8"/>
       <c r="T83" s="6"/>
       <c r="U83" s="6"/>
       <c r="V83" s="6"/>
-      <c r="W83" s="14"/>
-      <c r="X83" s="16"/>
-      <c r="Y83" s="6"/>
+      <c r="W83" s="6"/>
+      <c r="X83" s="14"/>
+      <c r="Y83" s="16"/>
+      <c r="Z83" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="W1:X1"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
@@ -2436,6 +2509,11 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sales order cluster by
</commit_message>
<xml_diff>
--- a/ad_works_lt/pipelines/tables.xlsx
+++ b/ad_works_lt/pipelines/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/python/databricks-patterns/ad_works_lt/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1E8F17-3A1A-A444-A0F9-96781CAC2665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F9A8D-F49F-EB48-BCBC-506C710930F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1240" windowWidth="38400" windowHeight="21100" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="82">
   <si>
     <t>stage</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>z_order_by</t>
-  </si>
-  <si>
-    <t>_load_date</t>
   </si>
   <si>
     <t>deltalake</t>
@@ -288,13 +285,16 @@
   </si>
   <si>
     <t>development</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -317,6 +317,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF22863A"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF032F62"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -379,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -441,16 +447,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -458,6 +464,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,9 +781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
   <dimension ref="A1:Z83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,32 +818,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
@@ -844,52 +851,52 @@
       <c r="M1" s="26"/>
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
       <c r="X1" s="27" t="s">
         <v>6</v>
       </c>
       <c r="Y1" s="27"/>
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
@@ -901,7 +908,7 @@
         <v>9</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>7</v>
@@ -913,7 +920,7 @@
         <v>9</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X2" s="11" t="s">
         <v>10</v>
@@ -930,10 +937,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
@@ -943,7 +950,7 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -974,20 +981,20 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1018,13 +1025,13 @@
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -1036,13 +1043,13 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1053,13 +1060,13 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1070,13 +1077,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1087,13 +1094,13 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1104,13 +1111,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1121,13 +1128,13 @@
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1138,13 +1145,13 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1155,13 +1162,13 @@
         <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1172,13 +1179,13 @@
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -1189,23 +1196,21 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="N15" s="3"/>
       <c r="O15" s="6">
         <v>30</v>
       </c>
@@ -1230,24 +1235,22 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="N16" s="3"/>
       <c r="O16" s="6">
         <v>30</v>
       </c>
@@ -1272,24 +1275,22 @@
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="N17" s="3"/>
       <c r="O17" s="6">
         <v>30</v>
       </c>
@@ -1314,24 +1315,22 @@
         <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="N18" s="3"/>
       <c r="O18" s="6">
         <v>30</v>
       </c>
@@ -1356,24 +1355,22 @@
         <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="N19" s="3"/>
       <c r="O19" s="6">
         <v>30</v>
       </c>
@@ -1398,24 +1395,22 @@
         <v>12</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="N20" s="3"/>
       <c r="O20" s="6">
         <v>30</v>
       </c>
@@ -1440,24 +1435,22 @@
         <v>12</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="N21" s="3"/>
       <c r="O21" s="6">
         <v>30</v>
       </c>
@@ -1482,24 +1475,22 @@
         <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="N22" s="3"/>
       <c r="O22" s="6">
         <v>30</v>
       </c>
@@ -1524,24 +1515,22 @@
         <v>12</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="N23" s="3"/>
       <c r="O23" s="6">
         <v>30</v>
       </c>
@@ -1566,24 +1555,22 @@
         <v>12</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="N24" s="3"/>
       <c r="O24" s="6">
         <v>30</v>
       </c>
@@ -1602,26 +1589,26 @@
     </row>
     <row r="25" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="6">
@@ -1642,26 +1629,26 @@
     </row>
     <row r="26" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N26" s="3"/>
       <c r="O26" s="6">
@@ -1682,26 +1669,26 @@
     </row>
     <row r="27" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="6">
@@ -1722,26 +1709,26 @@
     </row>
     <row r="28" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="6">
@@ -1762,26 +1749,26 @@
     </row>
     <row r="29" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="6">
@@ -1802,26 +1789,26 @@
     </row>
     <row r="30" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="6">
@@ -1842,26 +1829,26 @@
     </row>
     <row r="31" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="6">
@@ -1882,26 +1869,26 @@
     </row>
     <row r="32" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="6">
@@ -1922,26 +1909,29 @@
     </row>
     <row r="33" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="L33" s="28" t="s">
+        <v>81</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="6">
@@ -1962,26 +1952,26 @@
     </row>
     <row r="34" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="6">
@@ -2502,6 +2492,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
@@ -2509,11 +2504,6 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>